<commit_message>
Place order ASIA region
</commit_message>
<xml_diff>
--- a/src/test/resources/Files/Test_EMEA.xlsx
+++ b/src/test/resources/Files/Test_EMEA.xlsx
@@ -116,16 +116,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -146,10 +142,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -181,7 +177,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
+      <c r="A3" s="0" t="n">
         <v>666341</v>
       </c>
       <c r="B3" s="0" t="n">
@@ -189,27 +185,11 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
+      <c r="A4" s="0" t="n">
         <v>666606</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>12</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
-        <v>608765</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="n">
-        <v>607502</v>
-      </c>
-      <c r="B6" s="0" t="n">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>